<commit_message>
Data updated for TA, classifier for Vader is implemented
</commit_message>
<xml_diff>
--- a/ML_Data/first_50_dates/Calcs/Final results.xlsx
+++ b/ML_Data/first_50_dates/Calcs/Final results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923C3AF2-6E8B-4CBD-8D59-DBE5CBEDDC92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0446C6-8085-43B9-AB3F-DB099D0ED691}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2477" yWindow="2537" windowWidth="17589" windowHeight="10989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -171,11 +171,188 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -183,7 +360,9 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -192,10 +371,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -209,116 +388,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -331,29 +400,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,47 +706,47 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="13">
         <v>-3.7588512066153434E-3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="13">
         <v>-1.6233611113976476E-2</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="14">
         <v>1.9390316617164949E-2</v>
       </c>
       <c r="E2" s="15">
@@ -682,59 +754,59 @@
         <v>-2.0071523447562356E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="8">
         <v>0.27427033219897146</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="8">
         <v>0.25670496713833679</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>0.2647301032011935</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <f>AVERAGE(B3:D3)</f>
         <v>0.26523513417950056</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="6">
         <v>-0.11411730577160228</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>-0.17394731033348698</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="7">
         <v>-9.7771814741411944E-2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <f>AVERAGE(B4:D4)</f>
         <v>-0.12861214361550041</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="11">
         <f>AVERAGE(B2:B4)</f>
         <v>5.2131391740251276E-2</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="11">
         <f>AVERAGE(C2:C4)</f>
         <v>2.2174681896957777E-2</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="12">
         <f>AVERAGE(D2:D4)</f>
         <v>6.2116201692315499E-2</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>